<commit_message>
Update with migrations and initial seeding templates
</commit_message>
<xml_diff>
--- a/assets/Data Modeling.xlsx
+++ b/assets/Data Modeling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanthomas/Documents/lambda-school/repos/personal-projects/burning-heart/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanthomas/Documents/lambda-school/repos/personal-projects/burning-heart/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746DE15B-743F-8D4A-B504-D93DE56285D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3147A7-2EE7-D448-AD94-D6777E795DA4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27620" windowHeight="28340" xr2:uid="{269864E8-544A-794B-94B4-1941015625B3}"/>
+    <workbookView xWindow="53560" yWindow="8260" windowWidth="27620" windowHeight="20540" xr2:uid="{269864E8-544A-794B-94B4-1941015625B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,31 +420,52 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -463,27 +484,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -803,7 +803,7 @@
   <dimension ref="B2:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="D22" sqref="D21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -818,682 +818,682 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="17" customHeight="1">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="15"/>
+      <c r="E2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="2:8" ht="11" customHeight="1">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>1</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="13">
         <v>5.88</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>1</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="13">
         <v>30.29</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>4</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>3</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="13">
         <v>15.47</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>6</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>4</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="13">
         <v>3.2</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>8</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>5</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="13">
         <v>10</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>2</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>6</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="13">
         <v>19</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>3</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>7</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="13">
         <v>28</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>4</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>8</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>8</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="13">
         <v>4.3499999999999996</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>1</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>9</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="13">
         <v>2.9</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>5</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>10</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>10</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="13">
         <v>30.48</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>1</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>11</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>11</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="13">
         <v>20.47</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>4</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>12</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>12</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="13">
         <v>41.94</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>9</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>13</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>13</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="13">
         <v>28.69</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>14</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>14</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>14</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="13">
         <v>2.34</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>15</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>15</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>15</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="13">
         <v>46</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>13</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>16</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>16</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="13">
         <v>75.38</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>1</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>17</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>17</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="13">
         <v>1.01</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>13</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>18</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>18</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="13">
         <v>874.28</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>18</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>19</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>19</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="13">
         <v>5.43</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>18</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>20</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>20</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="13">
         <v>103.42</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>19</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>21</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>21</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="13">
         <v>67.11</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>9</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:8">
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>22</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>22</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="13">
         <v>48.32</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>2</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:8">
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>23</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>23</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="13">
         <v>32.450000000000003</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>23</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:8">
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>24</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>24</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="13">
         <v>68.38</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>24</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>25</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>25</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="13">
         <v>11</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>24</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>26</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>26</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="13">
         <v>47.37</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="6">
         <v>28</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>27</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>27</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="13">
         <v>69.23</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>27</v>
       </c>
-      <c r="H31" s="5">
+      <c r="H31" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <v>28</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>28</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="13">
         <v>23.69</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="6">
         <v>29</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>29</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
         <v>29</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="13">
         <v>18.45</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="6">
         <v>31</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <v>30</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>30</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="13">
         <v>23.14</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <v>30</v>
       </c>
-      <c r="H34" s="5">
+      <c r="H34" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:8">
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>31</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>31</v>
       </c>
-      <c r="F35" s="21">
+      <c r="F35" s="13">
         <v>23.45</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="6">
         <v>32</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H35" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="2:8">
-      <c r="B36" s="8">
+      <c r="B36" s="7">
         <v>32</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="7">
         <v>32</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="14">
         <v>9.7799999999999994</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="7">
         <v>13</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="7">
         <v>4</v>
       </c>
     </row>
@@ -1501,103 +1501,103 @@
     <row r="40" spans="2:8" ht="17" customHeight="1"/>
     <row r="41" spans="2:8" ht="17" customHeight="1"/>
     <row r="43" spans="2:8">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
     </row>
     <row r="44" spans="2:8">
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
     </row>
     <row r="45" spans="2:8">
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="46" spans="2:8">
-      <c r="B46" s="6">
+      <c r="B46" s="5">
         <v>1</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="2:8">
-      <c r="B47" s="7">
+      <c r="B47" s="6">
         <v>2</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="48" spans="2:8">
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <v>3</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="49" spans="2:6">
-      <c r="B49" s="8">
+      <c r="B49" s="7">
         <v>4</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="8" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Build out migrations + seeding data and create initial DB
</commit_message>
<xml_diff>
--- a/assets/Data Modeling.xlsx
+++ b/assets/Data Modeling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanthomas/Documents/lambda-school/repos/personal-projects/burning-heart/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3147A7-2EE7-D448-AD94-D6777E795DA4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE64FBC9-D437-5F4C-A62F-15CDB6362210}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53560" yWindow="8260" windowWidth="27620" windowHeight="20540" xr2:uid="{269864E8-544A-794B-94B4-1941015625B3}"/>
+    <workbookView xWindow="51200" yWindow="8260" windowWidth="33580" windowHeight="20540" xr2:uid="{269864E8-544A-794B-94B4-1941015625B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Charities</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Food for the Poor</t>
   </si>
   <si>
-    <t>person_id (FK)</t>
-  </si>
-  <si>
     <t>Users</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Samaritan's Purse</t>
   </si>
   <si>
-    <t>Luterhan Services in America</t>
-  </si>
-  <si>
     <t>American Cancer Society</t>
   </si>
   <si>
@@ -120,18 +114,12 @@
     <t>American Civil Liberties Union and Foundation</t>
   </si>
   <si>
-    <t>Nathan Thomas</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
     <t>asdfasdf</t>
   </si>
   <si>
-    <t>nate</t>
-  </si>
-  <si>
     <t>Veronica</t>
   </si>
   <si>
@@ -193,6 +181,21 @@
   </si>
   <si>
     <t>American Kidney Fund</t>
+  </si>
+  <si>
+    <t>Lutheran Services in America</t>
+  </si>
+  <si>
+    <t>user_id (FK)</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>nwthomas</t>
   </si>
 </sst>
 </file>
@@ -802,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F1E224-22A0-5D46-BF65-5A744163FA9F}">
   <dimension ref="B2:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D21:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -839,22 +842,22 @@
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:8">
@@ -1082,7 +1085,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="6">
         <v>12</v>
@@ -1102,7 +1105,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="6">
         <v>13</v>
@@ -1122,7 +1125,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E18" s="6">
         <v>14</v>
@@ -1142,7 +1145,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" s="6">
         <v>15</v>
@@ -1162,7 +1165,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="6">
         <v>16</v>
@@ -1182,7 +1185,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" s="6">
         <v>17</v>
@@ -1202,7 +1205,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" s="6">
         <v>18</v>
@@ -1222,7 +1225,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E23" s="6">
         <v>19</v>
@@ -1242,7 +1245,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E24" s="6">
         <v>20</v>
@@ -1262,7 +1265,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E25" s="6">
         <v>21</v>
@@ -1282,7 +1285,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E26" s="6">
         <v>22</v>
@@ -1302,7 +1305,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E27" s="6">
         <v>23</v>
@@ -1322,7 +1325,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E28" s="6">
         <v>24</v>
@@ -1342,7 +1345,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E29" s="6">
         <v>25</v>
@@ -1362,7 +1365,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6">
         <v>26</v>
@@ -1382,7 +1385,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E31" s="6">
         <v>27</v>
@@ -1402,7 +1405,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E32" s="6">
         <v>28</v>
@@ -1422,7 +1425,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E33" s="6">
         <v>29</v>
@@ -1442,7 +1445,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E34" s="6">
         <v>30</v>
@@ -1462,7 +1465,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E35" s="6">
         <v>31</v>
@@ -1482,7 +1485,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E36" s="7">
         <v>32</v>
@@ -1502,7 +1505,7 @@
     <row r="41" spans="2:8" ht="17" customHeight="1"/>
     <row r="43" spans="2:8">
       <c r="B43" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
@@ -1518,19 +1521,19 @@
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="2:8">
@@ -1538,16 +1541,16 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="2:8">
@@ -1555,16 +1558,16 @@
         <v>2</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="2:8">
@@ -1572,16 +1575,16 @@
         <v>3</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="F48" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -1589,16 +1592,16 @@
         <v>4</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>